<commit_message>
feat: add turnover rate, holdings information
</commit_message>
<xml_diff>
--- a/templates/template1.xlsx
+++ b/templates/template1.xlsx
@@ -14,9 +14,11 @@
     <sheet name="数据源-risk" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="数据源-manager" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="数据源-score" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="数据源-turnoverAndCentralization" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="数据源-top10Holdings" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">基金!$A$3:$AO$4</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">基金!$A$3:$AR$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="94">
   <si>
     <t xml:space="preserve">基本信息</t>
   </si>
@@ -204,6 +206,15 @@
     <t xml:space="preserve">成立来</t>
   </si>
   <si>
+    <t xml:space="preserve">前十持仓占比</t>
+  </si>
+  <si>
+    <t xml:space="preserve">前十持仓股票</t>
+  </si>
+  <si>
+    <t xml:space="preserve">换手率</t>
+  </si>
+  <si>
     <t xml:space="preserve">3年收益波动比</t>
   </si>
   <si>
@@ -802,6 +813,12 @@
   </si>
   <si>
     <t xml:space="preserve">晨星</t>
+  </si>
+  <si>
+    <t xml:space="preserve">前十持仓集中度</t>
+  </si>
+  <si>
+    <t xml:space="preserve">前十重仓股票</t>
   </si>
 </sst>
 </file>
@@ -1031,11 +1048,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1231,9 +1248,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="25" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="28" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="12.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1015" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1290,13 +1310,13 @@
       <c r="AK1" s="5"/>
       <c r="AL1" s="5"/>
       <c r="AM1" s="5"/>
-      <c r="AN1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AO1" s="5"/>
-      <c r="AMA1" s="0"/>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="0"/>
+      <c r="AT1" s="0"/>
+      <c r="AU1" s="0"/>
       <c r="AMD1" s="0"/>
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
@@ -1419,11 +1439,20 @@
       <c r="AM2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
-      <c r="AMA2" s="0"/>
-      <c r="AMB2" s="0"/>
-      <c r="AMC2" s="0"/>
+      <c r="AN2" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO2" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP2" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="0"/>
+      <c r="AT2" s="0"/>
+      <c r="AU2" s="0"/>
       <c r="AMD2" s="0"/>
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
@@ -1550,15 +1579,24 @@
       <c r="AM3" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AN3" s="11" t="s">
+      <c r="AN3" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AO3" s="11" t="s">
+      <c r="AO3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="AMA3" s="0"/>
-      <c r="AMB3" s="0"/>
-      <c r="AMC3" s="0"/>
+      <c r="AP3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS3" s="0"/>
+      <c r="AT3" s="0"/>
+      <c r="AU3" s="0"/>
       <c r="AMD3" s="0"/>
       <c r="AME3" s="0"/>
       <c r="AMF3" s="0"/>
@@ -1569,7 +1607,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" s="16" t="e">
         <f aca="false">VLOOKUP($A4,'数据源-basic'!$A:$L,B$2, 1)</f>
@@ -1717,17 +1755,29 @@
         <f aca="false">VLOOKUP($A4,'数据源-history'!$A:$K, AM$2, 1)</f>
         <v>#N/A</v>
       </c>
-      <c r="AN4" s="22" t="e">
+      <c r="AN4" s="3" t="e">
+        <f aca="false">VLOOKUP($A4,'数据源-turnoverAndCentralization'!$A:$C, AN$2,1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AO4" s="3" t="e">
+        <f aca="false">VLOOKUP($A4,'数据源-top10Holdings'!$A:$C, AO$2,1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AP4" s="3" t="e">
+        <f aca="false">VLOOKUP($A4,'数据源-turnoverAndCentralization'!$A:$C, AP$2,1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AQ4" s="22" t="e">
         <f aca="false">ROUND(AK4/X4, 2)</f>
         <v>#N/A</v>
       </c>
-      <c r="AO4" s="20" t="e">
+      <c r="AR4" s="20" t="e">
         <f aca="false">ROUND(AK4/3,4)</f>
         <v>#N/A</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AO4"/>
+  <autoFilter ref="A3:AR4"/>
   <mergeCells count="8">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
@@ -1736,7 +1786,7 @@
     <mergeCell ref="Q1:U1"/>
     <mergeCell ref="V1:AC1"/>
     <mergeCell ref="AD1:AM1"/>
-    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="V4:X4">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
@@ -1772,7 +1822,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1780,7 +1830,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.79"/>
@@ -1793,48 +1843,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="24" t="s">
+      <c r="D1" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" s="24" t="s">
+      <c r="G1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="J1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1867,37 +1910,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="24" t="s">
+      <c r="A1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="F1" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="G1" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="H1" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="25" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1933,31 +1976,31 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="24" t="s">
+      <c r="A1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="E1" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1991,16 +2034,16 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="24" t="s">
+      <c r="A1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="24" t="s">
+      <c r="C1" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2035,23 +2078,98 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="24" t="s">
+      <c r="A1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>88</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.98"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="141.35"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>